<commit_message>
added a file with the steps for the arduino code
</commit_message>
<xml_diff>
--- a/Teensy mapping.xlsx
+++ b/Teensy mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Teensy motor</t>
   </si>
@@ -36,6 +36,57 @@
   </si>
   <si>
     <t>task</t>
+  </si>
+  <si>
+    <t>move motor forward</t>
+  </si>
+  <si>
+    <t>move motor back</t>
+  </si>
+  <si>
+    <t>list of commands needed (output)</t>
+  </si>
+  <si>
+    <t>present Aluminum</t>
+  </si>
+  <si>
+    <t>present Attenuated</t>
+  </si>
+  <si>
+    <t>present no Object</t>
+  </si>
+  <si>
+    <t>Catch trail</t>
+  </si>
+  <si>
+    <t>list of commands needed (input)</t>
+  </si>
+  <si>
+    <t>motor at whisker</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>lickport</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>motor at start point</t>
+  </si>
+  <si>
+    <t>motor at object</t>
+  </si>
+  <si>
+    <t>object type pulses</t>
   </si>
 </sst>
 </file>
@@ -51,12 +102,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -71,8 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -364,9 +443,11 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,157 +460,281 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>23</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>22</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>21</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>20</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>19</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>18</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>16</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>8</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>7</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>6</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>5</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3">
         <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated teensy mapping for aluminum, saving before adding video write
</commit_message>
<xml_diff>
--- a/Teensy mapping.xlsx
+++ b/Teensy mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
   <si>
     <t>Teensy control</t>
   </si>
@@ -153,7 +153,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,12 +198,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor rgb="FF808000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFE699"/>
       </patternFill>
@@ -236,6 +230,18 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor rgb="FF3366FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FF808000"/>
       </patternFill>
     </fill>
   </fills>
@@ -368,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -392,58 +398,60 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +803,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,16 +817,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="43" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
@@ -829,20 +837,20 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47">
+      <c r="A2" s="44">
         <v>0</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="47">
+      <c r="A3" s="44">
         <v>1</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="46"/>
       <c r="H3" t="s">
         <v>6</v>
       </c>
@@ -851,14 +859,14 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="50">
+      <c r="A4" s="47">
         <v>2</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="48">
         <v>23</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="52"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="49"/>
       <c r="H4" t="s">
         <v>8</v>
       </c>
@@ -867,14 +875,14 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53">
+      <c r="A5" s="50">
         <v>3</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="51">
         <v>22</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
       <c r="H5" t="s">
         <v>10</v>
       </c>
@@ -883,19 +891,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="64">
+      <c r="A6" s="61">
         <v>4</v>
       </c>
-      <c r="B6" s="65">
+      <c r="B6" s="62">
         <v>21</v>
       </c>
-      <c r="C6" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="66" t="str">
-        <f>D52</f>
-        <v>Aluminum</v>
-      </c>
+      <c r="C6" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="63"/>
       <c r="H6" t="s">
         <v>12</v>
       </c>
@@ -904,16 +909,16 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="67">
+      <c r="A7" s="64">
         <v>5</v>
       </c>
-      <c r="B7" s="68">
+      <c r="B7" s="65">
         <v>20</v>
       </c>
-      <c r="C7" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="69" t="str">
+      <c r="C7" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="66" t="str">
         <f>D51</f>
         <v>Attenuated</v>
       </c>
@@ -922,16 +927,16 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="67">
+      <c r="A8" s="64">
         <v>6</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="65">
         <v>19</v>
       </c>
-      <c r="C8" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="69" t="str">
+      <c r="C8" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="66" t="str">
         <f>D50</f>
         <v>No Object</v>
       </c>
@@ -940,259 +945,261 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="67">
+      <c r="A9" s="64">
         <v>7</v>
       </c>
-      <c r="B9" s="68">
-        <v>18</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="69" t="str">
+      <c r="B9" s="65">
+        <v>18</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="66" t="str">
         <f>D49</f>
         <v>Catch trail</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="70">
+      <c r="A10" s="67">
         <v>8</v>
       </c>
-      <c r="B10" s="71">
-        <v>17</v>
-      </c>
-      <c r="C10" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="72" t="str">
+      <c r="B10" s="68">
+        <v>17</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="69" t="str">
         <f>D48</f>
         <v>move motor forward</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="53">
+      <c r="A11" s="50">
         <v>9</v>
       </c>
-      <c r="B11" s="56">
+      <c r="B11" s="53">
         <v>16</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="55"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="47">
+      <c r="A12" s="44">
         <v>10</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="46"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="47">
+      <c r="A13" s="44">
         <v>11</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47">
+      <c r="A14" s="44">
         <v>12</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="46"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73">
+      <c r="A15" s="70">
         <v>13</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="74"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="71"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="57">
+      <c r="A16" s="72">
         <v>14</v>
       </c>
-      <c r="B16" s="58">
+      <c r="B16" s="73">
         <v>11</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="59"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="74" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="57">
+      <c r="A17" s="54">
         <v>15</v>
       </c>
-      <c r="B17" s="58">
+      <c r="B17" s="55">
         <v>10</v>
       </c>
-      <c r="C17" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="59" t="str">
+      <c r="C17" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="56" t="str">
         <f>D41</f>
         <v>Motor at position</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="57">
+      <c r="A18" s="54">
         <v>16</v>
       </c>
-      <c r="B18" s="58">
+      <c r="B18" s="55">
         <v>9</v>
       </c>
-      <c r="C18" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="59" t="str">
+      <c r="C18" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="56" t="str">
         <f>D40</f>
         <v>R_object</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="57">
-        <v>17</v>
-      </c>
-      <c r="B19" s="58">
+      <c r="A19" s="54">
+        <v>17</v>
+      </c>
+      <c r="B19" s="55">
         <v>8</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="59" t="str">
+      <c r="C19" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="56" t="str">
         <f>D39</f>
         <v>R_aluminum</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="60">
-        <v>18</v>
-      </c>
-      <c r="B20" s="61">
+      <c r="A20" s="57">
+        <v>18</v>
+      </c>
+      <c r="B20" s="58">
         <v>7</v>
       </c>
-      <c r="C20" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="59" t="str">
+      <c r="C20" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="56" t="str">
         <f>D38</f>
         <v>R_attenuated</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="60">
+      <c r="A21" s="57">
         <v>19</v>
       </c>
-      <c r="B21" s="61">
+      <c r="B21" s="58">
         <v>6</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="59" t="str">
+      <c r="C21" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="56" t="str">
         <f>D37</f>
         <v>R_NON</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="47">
+      <c r="A22" s="44">
         <v>20</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="45">
         <v>5</v>
       </c>
-      <c r="C22" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="49" t="str">
+      <c r="C22" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="46" t="str">
         <f>D36</f>
         <v>Catch at position</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="47">
+      <c r="A23" s="44">
         <v>21</v>
       </c>
-      <c r="B23" s="48">
+      <c r="B23" s="45">
         <v>4</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="47">
+      <c r="A24" s="44">
         <v>22</v>
       </c>
-      <c r="B24" s="48">
+      <c r="B24" s="45">
         <v>3</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="73">
+      <c r="A25" s="70">
         <v>23</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="74" t="s">
+      <c r="C25" s="42"/>
+      <c r="D25" s="71" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="25"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
+      <c r="A31" s="26">
         <v>0</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="31"/>
+      <c r="C31" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="28"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="32">
+      <c r="A32" s="29">
         <v>1</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="34"/>
+      <c r="C32" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35">
+      <c r="A33" s="32">
         <v>2</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="37"/>
+      <c r="C33" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="34"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1218,13 +1225,13 @@
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="38">
+      <c r="A36" s="35">
         <v>5</v>
       </c>
-      <c r="B36" s="39">
+      <c r="B36" s="36">
         <v>20</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="37" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -1291,28 +1298,30 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="41">
+      <c r="A41" s="38">
         <v>10</v>
       </c>
-      <c r="B41" s="42">
+      <c r="B41" s="39">
         <v>15</v>
       </c>
-      <c r="C41" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="43" t="s">
+      <c r="C41" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="40" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="23">
+      <c r="A42" s="75">
         <v>11</v>
       </c>
-      <c r="B42" s="24">
+      <c r="B42" s="76">
         <v>14</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="25"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17">
@@ -1323,50 +1332,50 @@
       <c r="D43" s="19"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="29">
+      <c r="A44" s="26">
         <v>13</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="31"/>
+      <c r="C44" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="28"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="32">
+      <c r="A45" s="29">
         <v>14</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="34"/>
+      <c r="C45" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="31"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="35">
+      <c r="A46" s="32">
         <v>15</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D46" s="37"/>
+      <c r="C46" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="34"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="62">
+      <c r="A47" s="59">
         <v>16</v>
       </c>
-      <c r="B47" s="63">
+      <c r="B47" s="60">
         <v>9</v>
       </c>
-      <c r="C47" s="63"/>
-      <c r="D47" s="28"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="25"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
@@ -1434,9 +1443,7 @@
       <c r="C52" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D52" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="D52" s="11"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">

</xml_diff>

<commit_message>
changed the motor going back to a new command, added reset at beginig of trial to make sure motor goes back
</commit_message>
<xml_diff>
--- a/Teensy mapping.xlsx
+++ b/Teensy mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Teensy control</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Water prize</t>
+  </si>
+  <si>
+    <t>R_reset</t>
   </si>
 </sst>
 </file>
@@ -802,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,8 +1130,12 @@
       <c r="B23" s="45">
         <v>4</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
+      <c r="C23" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44">
@@ -1220,8 +1227,12 @@
       <c r="B35" s="21">
         <v>21</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="22"/>
+      <c r="C35" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>38</v>
+      </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
minor changes to teensy mapping
</commit_message>
<xml_diff>
--- a/Teensy mapping.xlsx
+++ b/Teensy mapping.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Teensy control</t>
   </si>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,9 @@
         <v>22</v>
       </c>
       <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
+      <c r="D5" s="52" t="s">
+        <v>30</v>
+      </c>
       <c r="H5" t="s">
         <v>10</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="56" t="str">
-        <f>D41</f>
+        <f>D34</f>
         <v>Motor at position</v>
       </c>
     </row>
@@ -1209,7 +1211,7 @@
       <c r="D33" s="34"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20">
         <v>3</v>
       </c>
@@ -1217,7 +1219,9 @@
         <v>22</v>
       </c>
       <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
+      <c r="D34" s="40" t="s">
+        <v>30</v>
+      </c>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1317,9 +1321,6 @@
       </c>
       <c r="C41" s="39" t="s">
         <v>18</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>